<commit_message>
Forgot to save interpolation parameters excel sheet - saved it so other peeps can have all values.
</commit_message>
<xml_diff>
--- a/Lab 4/interpolation parameters.xlsx
+++ b/Lab 4/interpolation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\enel453Project\Lab 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6DC36C2-0103-4163-8A8C-15D5BA0EC098}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECE1D5E-96D4-4733-A46A-78A0D63D4609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A872511F-DB86-4839-8110-A594A404BEB4}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{A872511F-DB86-4839-8110-A594A404BEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>interpolation parameters</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>blinking</t>
+  </si>
+  <si>
+    <t>xmin</t>
+  </si>
+  <si>
+    <t>xmax</t>
+  </si>
+  <si>
+    <t>ymin</t>
+  </si>
+  <si>
+    <t>ymax</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>fmax</t>
+  </si>
+  <si>
+    <t>fmin</t>
+  </si>
+  <si>
+    <t>kHz</t>
+  </si>
+  <si>
+    <t>clock cycles</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>clk freq</t>
+  </si>
+  <si>
+    <t>PWM freq</t>
+  </si>
+  <si>
+    <t>fmax factor</t>
+  </si>
+  <si>
+    <t>fmin factor</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>clk period</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>initial pwm period</t>
+  </si>
+  <si>
+    <t>expect pwm period</t>
   </si>
 </sst>
 </file>
@@ -388,15 +457,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F1384E-14B6-45D4-8574-4294083B3320}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.5</v>
+      </c>
+      <c r="C2">
+        <f>B2</f>
+        <v>3.5</v>
+      </c>
+      <c r="D2">
+        <f>C2</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <f>B3</f>
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <f>C3</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>511</v>
+      </c>
+      <c r="C4">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>24462</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>489237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <f>(B5-B4)/(B3-B2)</f>
+        <v>-14</v>
+      </c>
+      <c r="C6">
+        <f>(C5-C4)/(C3-C2)</f>
+        <v>-1.0136986301369864</v>
+      </c>
+      <c r="D6">
+        <f>(D5-D4)/(D3-D2)</f>
+        <v>12733.561643835616</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>B4-B2*B6</f>
+        <v>560</v>
+      </c>
+      <c r="C7">
+        <f>C4-C2*C6</f>
+        <v>52.547945205479451</v>
+      </c>
+      <c r="D7">
+        <f>D4-D2*D6</f>
+        <v>-20105.465753424651</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <f>LOG(D5,2)-1</f>
+        <v>17.900173990521985</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>511</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <f>C11</f>
+        <v>511</v>
+      </c>
+      <c r="G11" t="str">
+        <f>D11</f>
+        <v>clock cycles</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>50000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <f>C12*1000</f>
+        <v>50000000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <f>C12/C11</f>
+        <v>97.847358121330728</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <f>C13*1000</f>
+        <v>97847.358121330733</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <f>C13/C9</f>
+        <v>12.230919765166341</v>
+      </c>
+      <c r="F14">
+        <f>F13/F9</f>
+        <v>24461.839530332683</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <f>C13/C10</f>
+        <v>48.923679060665364</v>
+      </c>
+      <c r="F15">
+        <f>F13/F10</f>
+        <v>489236.79060665367</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0.02</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <f>C12</f>
+        <v>50000</v>
+      </c>
+      <c r="D18" t="str">
+        <f>D12</f>
+        <v>kHz</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18">
+        <v>1.0240000000000001E-2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <f>1/C18</f>
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <f>C17/C19</f>
+        <v>999.99999999999989</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <f>H19*H18</f>
+        <v>3.0720000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added LUT-based implementation for blinking and PWM instead of the interpolator, though the interpolator will still be available. Added math to calculate the LUT values to the voltage2distance scratch spreadsheet and the interpolation parameters spreadsheet.
</commit_message>
<xml_diff>
--- a/Lab 4/interpolation parameters.xlsx
+++ b/Lab 4/interpolation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\enel453Project\Lab 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECE1D5E-96D4-4733-A46A-78A0D63D4609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF972B1-50AC-426B-9B5E-5BA278CBC4D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{A872511F-DB86-4839-8110-A594A404BEB4}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8976" xr2:uid="{A872511F-DB86-4839-8110-A594A404BEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,15 +481,15 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <f>B2</f>
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <f>C2</f>
-        <v>3.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -497,15 +497,15 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="C3">
         <f>B3</f>
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="D3">
         <f>C3</f>
-        <v>40</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -542,15 +542,15 @@
       </c>
       <c r="B6">
         <f>(B5-B4)/(B3-B2)</f>
-        <v>-14</v>
+        <v>-1.4</v>
       </c>
       <c r="C6">
         <f>(C5-C4)/(C3-C2)</f>
-        <v>-1.0136986301369864</v>
+        <v>-0.10136986301369863</v>
       </c>
       <c r="D6">
         <f>(D5-D4)/(D3-D2)</f>
-        <v>12733.561643835616</v>
+        <v>1273.3561643835617</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -567,7 +567,7 @@
       </c>
       <c r="D7">
         <f>D4-D2*D6</f>
-        <v>-20105.465753424651</v>
+        <v>-20105.465753424658</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added lab 4 7 segment display behaviour.
</commit_message>
<xml_diff>
--- a/Lab 4/interpolation parameters.xlsx
+++ b/Lab 4/interpolation parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\enel453Project\Lab 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF972B1-50AC-426B-9B5E-5BA278CBC4D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B7052A-D8C5-4E17-A744-6193AA2C86FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8976" xr2:uid="{A872511F-DB86-4839-8110-A594A404BEB4}"/>
+    <workbookView xWindow="-27840" yWindow="960" windowWidth="21600" windowHeight="11325" xr2:uid="{A872511F-DB86-4839-8110-A594A404BEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>